<commit_message>
3.0.11: Implement menuItemDescription option, thant can specify item for description.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentTask.xlsx
+++ b/meta/program/BlancoVueComponentTask.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999EFE3-1EBD-6A4A-BAA9-D895AA22737D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D29543-C86F-DD4E-96A5-1676D30137C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="3320" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2720" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anttask" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -621,6 +621,36 @@
     </rPh>
     <rPh sb="73" eb="75">
       <t xml:space="preserve">サクセイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>menuItemDescription</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>"description"</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>MenuItem の description に割り当てる項目名を指定します。項目名にはClassStructure で定義しているプロパティ名を使用します。</t>
+    <rPh sb="29" eb="32">
+      <t xml:space="preserve">コウモクメイヲ </t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t xml:space="preserve">シテイシマス。 </t>
+    </rPh>
+    <rPh sb="39" eb="42">
+      <t xml:space="preserve">コウモクメイニ </t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t xml:space="preserve">メイヲ </t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t xml:space="preserve">シヨウシマス。 </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1209,6 +1239,17 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1240,17 +1281,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1619,10 +1649,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30:I30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1668,10 +1698,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="6" t="s">
         <v>49</v>
       </c>
@@ -1680,10 +1710,10 @@
       <c r="F6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="61"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="6" t="s">
         <v>50</v>
       </c>
@@ -1694,10 +1724,10 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="61"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="6" t="s">
         <v>51</v>
       </c>
@@ -1708,10 +1738,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="61"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1742,38 +1772,38 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
       <c r="A14" s="36">
@@ -1789,12 +1819,12 @@
         <v>13</v>
       </c>
       <c r="E14" s="40"/>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="64"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="69"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
       <c r="A15" s="41">
@@ -1811,12 +1841,12 @@
       <c r="E15" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="68" t="s">
+      <c r="F15" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="70"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="75"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="41">
@@ -1833,12 +1863,12 @@
       <c r="E16" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="71" t="s">
+      <c r="F16" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="70"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="75"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="41">
@@ -1941,12 +1971,12 @@
       <c r="E21" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="76"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:10" ht="56" customHeight="1">
       <c r="A22" s="41">
@@ -2035,7 +2065,7 @@
     </row>
     <row r="26" spans="1:10" ht="65" customHeight="1">
       <c r="A26" s="41">
-        <f t="shared" ref="A26:A29" si="2">A25+1</f>
+        <f t="shared" ref="A26:A30" si="2">A25+1</f>
         <v>13</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -2116,26 +2146,37 @@
       <c r="I29" s="60"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="41"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="34"/>
+      <c r="A30" s="41">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="58"/>
+      <c r="E30" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>69</v>
+      </c>
       <c r="G30" s="59"/>
       <c r="H30" s="59"/>
       <c r="I30" s="60"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="17"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="18"/>
       <c r="C31" s="34"/>
       <c r="D31" s="19"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="22"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="17"/>
@@ -2160,26 +2201,31 @@
       <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="28"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F12:I13"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F21:I21"/>
+  <mergeCells count="24">
     <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="A6:B6"/>
@@ -2195,17 +2241,24 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F21:I21"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F50" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D23 D25:D34" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D23 D25:D35" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C23 C25:C34" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C23 C25:C35" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
3.0.17 Implement strictNullable option. Default false. on true, depend " | undefined | null" to type of nullable properties.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentTask.xlsx
+++ b/meta/program/BlancoVueComponentTask.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F2B9F7-8295-9648-9C2C-DC838D6DA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09A1497-509E-C64E-BD1C-ECDCCB8BA609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16120" yWindow="2420" windowWidth="28800" windowHeight="17500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anttask" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -701,6 +701,26 @@
     </rPh>
     <rPh sb="95" eb="97">
       <t xml:space="preserve">シテイシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>strictNullable</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Nullable な property に対して、? の付与をやめて | undefined | null の定義を行う。false の場合は ? が付与されて | undefined のみ付与される。</t>
+    <rPh sb="7" eb="9">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シュツリョク</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1286,6 +1306,17 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1317,17 +1348,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1696,10 +1716,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:I32"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1745,10 +1765,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="60"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="6" t="s">
         <v>49</v>
       </c>
@@ -1757,10 +1777,10 @@
       <c r="F6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="60"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="6" t="s">
         <v>50</v>
       </c>
@@ -1771,10 +1791,10 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="60"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="6" t="s">
         <v>51</v>
       </c>
@@ -1785,10 +1805,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="60"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1819,38 +1839,38 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="64"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
       <c r="A14" s="36">
@@ -1866,12 +1886,12 @@
         <v>13</v>
       </c>
       <c r="E14" s="40"/>
-      <c r="F14" s="61" t="s">
+      <c r="F14" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="63"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
       <c r="A15" s="41">
@@ -1888,16 +1908,16 @@
       <c r="E15" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="67" t="s">
+      <c r="F15" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="69"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="74"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="41">
-        <f t="shared" ref="A16:A31" si="0">A15+1</f>
+        <f t="shared" ref="A16:A32" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="42" t="s">
@@ -1910,12 +1930,12 @@
       <c r="E16" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="70" t="s">
+      <c r="F16" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="69"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="74"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="41">
@@ -2018,12 +2038,12 @@
       <c r="E21" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="73" t="s">
+      <c r="F21" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="75"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="64"/>
     </row>
     <row r="22" spans="1:10" ht="56" customHeight="1">
       <c r="A22" s="41">
@@ -2235,37 +2255,48 @@
       <c r="I31" s="59"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="41"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="34"/>
+      <c r="A32" s="41">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="D32" s="19"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
+      <c r="E32" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="41"/>
       <c r="B33" s="18"/>
       <c r="C33" s="34"/>
       <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
+      <c r="E33" s="52"/>
       <c r="F33" s="57"/>
       <c r="G33" s="58"/>
       <c r="H33" s="58"/>
       <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="17"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="18"/>
       <c r="C34" s="34"/>
       <c r="D34" s="19"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="22"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="17"/>
@@ -2290,30 +2321,30 @@
       <c r="I36" s="22"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="28"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F12:I13"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="A6:B6"/>
@@ -2328,17 +2359,28 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F30:I30"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F53" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F54" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D23 D25:D37" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D23 D25:D38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C23 C25:C37" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C23 C25:C38" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>